<commit_message>
Product backlog update 04/30/2018
</commit_message>
<xml_diff>
--- a/docs/deliverable4/Getana_Deliverable_4_ProductBacklog.xlsx
+++ b/docs/deliverable4/Getana_Deliverable_4_ProductBacklog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="81">
   <si>
     <t>PRODUCT BACKLOG — DELIVERABLE 4</t>
   </si>
@@ -86,9 +86,6 @@
     <t>As a user, I want the app to tell me how much time is available until my next class begins, so that I can more easily fit unscheduled activities into my day without calculating myself the amount of time available until class begins.</t>
   </si>
   <si>
-    <t>M, 5</t>
-  </si>
-  <si>
     <t>As a user, I want the app to notify me with special messages when I am in danger of being late to class, based on the time the class begins and the travel time necessary to reach the building, so that I can afford to be distracted and do not have to constantly check the app.</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>As a user, I want the app to show me shortest paths which include bus routes, so that I can reach very far destinations on campus quickly.</t>
   </si>
   <si>
-    <t>L, 10</t>
-  </si>
-  <si>
     <t>← from presentation feedback</t>
   </si>
   <si>
@@ -263,7 +257,16 @@
     <t>As a user, I want to choose two classes loctions from a list and then the app show me the route between them on the map</t>
   </si>
   <si>
-    <t>H, 23</t>
+    <t>M, 10</t>
+  </si>
+  <si>
+    <t>L, 18</t>
+  </si>
+  <si>
+    <t>L, 23</t>
+  </si>
+  <si>
+    <t>H, 5</t>
   </si>
 </sst>
 </file>
@@ -831,7 +834,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -885,16 +888,16 @@
         <v>35</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -911,10 +914,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -931,7 +934,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>12</v>
@@ -951,7 +954,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>12</v>
@@ -971,7 +974,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>12</v>
@@ -991,7 +994,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>12</v>
@@ -1005,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>12</v>
@@ -1025,13 +1028,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>12</v>
@@ -1045,13 +1048,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>12</v>
@@ -1065,13 +1068,13 @@
         <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>12</v>
@@ -1085,13 +1088,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>12</v>
@@ -1100,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -1108,7 +1111,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
@@ -1128,13 +1131,13 @@
         <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>12</v>
@@ -1143,7 +1146,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -1151,7 +1154,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>10</v>
@@ -1172,7 +1175,7 @@
         <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>10</v>
@@ -1187,7 +1190,7 @@
         <v>7</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -1195,7 +1198,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>10</v>
@@ -1210,7 +1213,7 @@
         <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -1218,7 +1221,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>10</v>
@@ -1238,13 +1241,13 @@
         <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>12</v>
@@ -1258,13 +1261,13 @@
         <v>17</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>12</v>
@@ -1278,13 +1281,13 @@
         <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>12</v>
@@ -1293,7 +1296,7 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -1301,13 +1304,13 @@
         <v>20</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>12</v>
@@ -1321,13 +1324,13 @@
         <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>12</v>
@@ -1336,13 +1339,13 @@
         <v>5</v>
       </c>
       <c r="G28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1358,13 +1361,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F30">
         <v>3</v>
@@ -1375,13 +1378,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F31">
         <v>3</v>
@@ -1392,13 +1395,13 @@
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F32">
         <v>3</v>
@@ -1409,13 +1412,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -1426,19 +1429,19 @@
         <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F34">
         <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="39" x14ac:dyDescent="0.25">
@@ -1446,13 +1449,13 @@
         <v>19</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F35">
         <v>3</v>
@@ -1463,20 +1466,20 @@
         <v>24</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C36" s="5">
         <v>4</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F36" s="5">
         <v>6</v>
       </c>
       <c r="G36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1484,19 +1487,19 @@
         <v>30</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1504,13 +1507,13 @@
         <v>5</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38">
         <v>4</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F38">
         <v>4</v>
@@ -1521,13 +1524,13 @@
         <v>21</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C39">
         <v>5</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -1538,13 +1541,13 @@
         <v>8</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C40">
         <v>5</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1555,13 +1558,13 @@
         <v>9</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C41" s="5">
         <v>5</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -1572,13 +1575,13 @@
         <v>34</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" s="5">
         <v>4</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1593,19 +1596,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B44" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="E44" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="F44" s="16" t="s">
         <v>74</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update product backlog and sprint backlog for story 16
</commit_message>
<xml_diff>
--- a/docs/deliverable4/Getana_Deliverable_4_ProductBacklog.xlsx
+++ b/docs/deliverable4/Getana_Deliverable_4_ProductBacklog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuyon\Documents\GitHub\RaiderNAV\docs\deliverable4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>PRODUCT BACKLOG — DELIVERABLE 4</t>
   </si>
@@ -53,9 +48,6 @@
     <t>Story Points</t>
   </si>
   <si>
-    <t>As a user, I want to be able to arbitrarily add some other locations to the app and to my schedules, so that I can plan in regular lunch destinations or walks for exercise between classes.</t>
-  </si>
-  <si>
     <t>undecided</t>
   </si>
   <si>
@@ -263,16 +255,16 @@
     <t>L, 18</t>
   </si>
   <si>
-    <t>L, 23</t>
-  </si>
-  <si>
     <t>H, 5</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to arbitrarily add some other locations to the app, so that I can plan in meals.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -823,7 +815,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -834,7 +826,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -848,22 +840,22 @@
     <col min="7" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -883,499 +875,496 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>35</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>12</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12">
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
+    <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>23</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14">
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="5">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3" t="s">
+    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>26</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="5">
+      <c r="C18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18">
         <v>6</v>
       </c>
-      <c r="G17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="G18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19">
         <v>6</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20">
-        <v>6</v>
-      </c>
-      <c r="G20" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21">
-        <v>7</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="5">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29">
         <v>2</v>
       </c>
-      <c r="G26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>20</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="5">
-        <v>5</v>
-      </c>
-      <c r="G28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>58</v>
@@ -1384,15 +1373,15 @@
         <v>2</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>59</v>
@@ -1401,90 +1390,93 @@
         <v>2</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F34">
         <v>3</v>
       </c>
-      <c r="G34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="39" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>19</v>
+    </row>
+    <row r="35" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>24</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
+      <c r="C35" s="5">
+        <v>4</v>
+      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="F35" s="5">
+        <v>6</v>
+      </c>
+      <c r="G35" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>24</v>
+      <c r="A36">
+        <v>30</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36">
         <v>4</v>
       </c>
-      <c r="D36" s="5"/>
       <c r="E36" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="5">
-        <v>6</v>
+        <v>56</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>64</v>
@@ -1493,35 +1485,32 @@
         <v>4</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>57</v>
+        <v>5</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="F38">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>66</v>
@@ -1530,85 +1519,84 @@
         <v>5</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="5">
         <v>5</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C41" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="5">
-        <v>4</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>57</v>
+        <v>79</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B43" s="12"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B44" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="D44" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="E44" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="F44" s="16" t="s">
         <v>73</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>